<commit_message>
update code and results
</commit_message>
<xml_diff>
--- a/results/annex_reg_annual.xlsx
+++ b/results/annex_reg_annual.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ihzhang/Documents/GitHub/Municipal-Boundary-Changes/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBAD80CB-1560-2847-9DB0-80561756729A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18D4A3B-85C1-934E-A793-C28D9986909F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="21800" windowHeight="12240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="13120" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -65,13 +65,13 @@
     <t>logLik</t>
   </si>
   <si>
+    <t>VRA*2008</t>
+  </si>
+  <si>
+    <t>VRA*2009</t>
+  </si>
+  <si>
     <t>VRA*2010</t>
-  </si>
-  <si>
-    <t>VRA*2008</t>
-  </si>
-  <si>
-    <t>VRA*2009</t>
   </si>
   <si>
     <t>VRA*2011</t>
@@ -431,14 +431,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -486,125 +483,125 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>1.0026229536396E-2</v>
+        <v>6.6149040397870604E-3</v>
       </c>
       <c r="C2">
-        <v>1.02900852181409E-2</v>
+        <v>7.9034282797482095E-3</v>
       </c>
       <c r="D2">
-        <v>0.97435826077710697</v>
+        <v>0.83696641579415998</v>
       </c>
       <c r="E2">
-        <v>0.33588376865459502</v>
+        <v>0.407710991203248</v>
       </c>
       <c r="F2">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G2">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H2">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J2">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K2">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L2">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M2">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N2">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>9.8120159046599896E-3</v>
+        <v>9.3408701945182897E-3</v>
       </c>
       <c r="C3">
-        <v>1.4593021233760399E-2</v>
+        <v>1.0279146498665201E-2</v>
       </c>
       <c r="D3">
-        <v>0.67237727866524599</v>
+        <v>0.90872040745127003</v>
       </c>
       <c r="E3">
-        <v>0.50530786308415598</v>
+        <v>0.36907932466900201</v>
       </c>
       <c r="F3">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G3">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H3">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J3">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K3">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L3">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M3">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N3">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>1.1475874632343899E-3</v>
+        <v>-1.1903456839028E-3</v>
       </c>
       <c r="C4">
-        <v>7.1117292450581298E-3</v>
+        <v>6.3071416014677303E-3</v>
       </c>
       <c r="D4">
-        <v>0.16136546031077301</v>
+        <v>-0.18872981758104199</v>
       </c>
       <c r="E4">
-        <v>0.872638620810123</v>
+        <v>0.85128327710139795</v>
       </c>
       <c r="F4">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G4">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H4">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J4">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K4">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L4">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M4">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N4">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -612,40 +609,40 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>3.3862586782045902E-3</v>
+        <v>2.7366175827523301E-3</v>
       </c>
       <c r="C5">
-        <v>8.3255307071954301E-3</v>
+        <v>8.0592762048542106E-3</v>
       </c>
       <c r="D5">
-        <v>0.40673187059150201</v>
+        <v>0.339561210360805</v>
       </c>
       <c r="E5">
-        <v>0.68642850114604204</v>
+        <v>0.736008877314134</v>
       </c>
       <c r="F5">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G5">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H5">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J5">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K5">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L5">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M5">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N5">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -653,40 +650,40 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>3.3144936421146401E-3</v>
+        <v>2.3330084036496902E-3</v>
       </c>
       <c r="C6">
-        <v>7.1801829722925497E-3</v>
+        <v>7.1678043351502798E-3</v>
       </c>
       <c r="D6">
-        <v>0.46161687730032303</v>
+        <v>0.32548438748653102</v>
       </c>
       <c r="E6">
-        <v>0.64692064667813398</v>
+        <v>0.74655436720687096</v>
       </c>
       <c r="F6">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G6">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H6">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J6">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K6">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L6">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M6">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N6">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -694,40 +691,40 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>-1.6011616217757099E-3</v>
+        <v>-3.5946948887934701E-3</v>
       </c>
       <c r="C7">
-        <v>8.16174037312716E-3</v>
+        <v>7.82585987499731E-3</v>
       </c>
       <c r="D7">
-        <v>-0.19617894573657299</v>
+        <v>-0.45933545274406201</v>
       </c>
       <c r="E7">
-        <v>0.84548878034598496</v>
+        <v>0.64854345132457902</v>
       </c>
       <c r="F7">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G7">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H7">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J7">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K7">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L7">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M7">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N7">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -735,40 +732,40 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>3.3958498162951498E-3</v>
+        <v>3.6247695090147998E-3</v>
       </c>
       <c r="C8">
-        <v>7.7755063013482204E-3</v>
+        <v>7.6725716207913597E-3</v>
       </c>
       <c r="D8">
-        <v>0.43673680975685603</v>
+        <v>0.47243215028352298</v>
       </c>
       <c r="E8">
-        <v>0.66471080814262995</v>
+        <v>0.63925143415359997</v>
       </c>
       <c r="F8">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G8">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H8">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J8">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K8">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L8">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M8">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N8">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -776,40 +773,40 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>5.1938217471522701E-3</v>
+        <v>2.8199061318337098E-3</v>
       </c>
       <c r="C9">
-        <v>1.0204432925333601E-2</v>
+        <v>1.0072838225464001E-2</v>
       </c>
       <c r="D9">
-        <v>0.50897700883093899</v>
+        <v>0.27995149616371601</v>
       </c>
       <c r="E9">
-        <v>0.61363601254606603</v>
+        <v>0.78099425966426095</v>
       </c>
       <c r="F9">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G9">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H9">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J9">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K9">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L9">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M9">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N9">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -817,40 +814,40 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <v>4.9569352056653198E-3</v>
+        <v>4.7713211880812297E-3</v>
       </c>
       <c r="C10">
-        <v>7.4157024276855603E-3</v>
+        <v>7.58054062300952E-3</v>
       </c>
       <c r="D10">
-        <v>0.66843771766774895</v>
+        <v>0.62941700669720702</v>
       </c>
       <c r="E10">
-        <v>0.50779144236553497</v>
+        <v>0.532746126605388</v>
       </c>
       <c r="F10">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G10">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H10">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J10">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K10">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L10">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M10">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N10">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -858,40 +855,40 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <v>-1.2403239043752201E-3</v>
+        <v>-1.06797309195083E-3</v>
       </c>
       <c r="C11">
-        <v>8.2222734939748493E-3</v>
+        <v>8.5507297130116497E-3</v>
       </c>
       <c r="D11">
-        <v>-0.15084926392732001</v>
+        <v>-0.124898473907519</v>
       </c>
       <c r="E11">
-        <v>0.88087217512112204</v>
+        <v>0.90124551208853299</v>
       </c>
       <c r="F11">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G11">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H11">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J11">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K11">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L11">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M11">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N11">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -899,40 +896,40 @@
         <v>24</v>
       </c>
       <c r="B12">
-        <v>1.15837950727068E-2</v>
+        <v>7.3738560896559101E-3</v>
       </c>
       <c r="C12">
-        <v>8.5225043272328105E-3</v>
+        <v>9.0211602501267807E-3</v>
       </c>
       <c r="D12">
-        <v>1.3592008437815599</v>
+        <v>0.81739553285867805</v>
       </c>
       <c r="E12">
-        <v>0.18189123447684699</v>
+        <v>0.418668157608728</v>
       </c>
       <c r="F12">
-        <v>0.17584145744542501</v>
+        <v>0.17213590243073101</v>
       </c>
       <c r="G12">
-        <v>9.1875070953464602E-2</v>
+        <v>9.6769249543292898E-2</v>
       </c>
       <c r="H12">
-        <v>1.2604474077793101E-4</v>
+        <v>9.9909906637218895E-5</v>
       </c>
       <c r="J12">
-        <v>0.15954162381031101</v>
+        <v>0.160682718346258</v>
       </c>
       <c r="K12">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L12">
-        <v>-127561.54156886</v>
+        <v>-144453.28296797301</v>
       </c>
       <c r="M12">
-        <v>31538.9850006292</v>
+        <v>21644.108686584299</v>
       </c>
       <c r="N12">
-        <v>79610.7707844299</v>
+        <v>88537.641483986299</v>
       </c>
     </row>
   </sheetData>
@@ -945,14 +942,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.5" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1000,125 +994,125 @@
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B2">
-        <v>9.6890859519375306E-3</v>
+        <v>6.4780806834404204E-3</v>
       </c>
       <c r="C2">
-        <v>1.0239373028494E-2</v>
+        <v>7.9378950602303402E-3</v>
       </c>
       <c r="D2">
-        <v>0.94625773716563399</v>
+        <v>0.81609553090418896</v>
       </c>
       <c r="E2">
-        <v>0.34984343674021801</v>
+        <v>0.41940231537551798</v>
       </c>
       <c r="F2">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G2">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H2">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J2">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K2">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L2">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M2">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N2">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3">
-        <v>9.48848850345556E-3</v>
+        <v>9.1203528794646001E-3</v>
       </c>
       <c r="C3">
-        <v>1.45795895989462E-2</v>
+        <v>1.03047179647548E-2</v>
       </c>
       <c r="D3">
-        <v>0.650806282238658</v>
+        <v>0.88506574470635202</v>
       </c>
       <c r="E3">
-        <v>0.51898772846396701</v>
+        <v>0.38154564841150901</v>
       </c>
       <c r="F3">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G3">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H3">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J3">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K3">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L3">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M3">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N3">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4">
-        <v>8.11295190267288E-4</v>
+        <v>-1.3341497633208999E-3</v>
       </c>
       <c r="C4">
-        <v>7.03325384478053E-3</v>
+        <v>5.2123385180658198E-3</v>
       </c>
       <c r="D4">
-        <v>0.115351330717199</v>
+        <v>-0.25595992253702898</v>
       </c>
       <c r="E4">
-        <v>0.90875854023374103</v>
+        <v>0.79932706892092498</v>
       </c>
       <c r="F4">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G4">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H4">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J4">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K4">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L4">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M4">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N4">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
@@ -1126,40 +1120,40 @@
         <v>17</v>
       </c>
       <c r="B5">
-        <v>2.6330415505351201E-3</v>
+        <v>1.17298234187699E-3</v>
       </c>
       <c r="C5">
-        <v>8.1801730557548493E-3</v>
+        <v>6.7355520113234098E-3</v>
       </c>
       <c r="D5">
-        <v>0.32188091041457201</v>
+        <v>0.17414791540545399</v>
       </c>
       <c r="E5">
-        <v>0.74926190980821505</v>
+        <v>0.86265007403469796</v>
       </c>
       <c r="F5">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G5">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H5">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J5">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K5">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L5">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M5">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N5">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
@@ -1167,40 +1161,40 @@
         <v>18</v>
       </c>
       <c r="B6">
-        <v>2.6768663066018602E-3</v>
+        <v>8.7346062197472102E-4</v>
       </c>
       <c r="C6">
-        <v>6.9413311953242596E-3</v>
+        <v>5.9492346082914297E-3</v>
       </c>
       <c r="D6">
-        <v>0.38564163433161303</v>
+        <v>0.146818990926561</v>
       </c>
       <c r="E6">
-        <v>0.70185768490606004</v>
+        <v>0.88403123969452402</v>
       </c>
       <c r="F6">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G6">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H6">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J6">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K6">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L6">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M6">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N6">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.2">
@@ -1208,40 +1202,40 @@
         <v>19</v>
       </c>
       <c r="B7">
-        <v>-1.7947603421997701E-3</v>
+        <v>-4.2550411471408501E-3</v>
       </c>
       <c r="C7">
-        <v>8.1994497033383903E-3</v>
+        <v>6.6274636595691798E-3</v>
       </c>
       <c r="D7">
-        <v>-0.21888790188798099</v>
+        <v>-0.642031607521096</v>
       </c>
       <c r="E7">
-        <v>0.82787885937308703</v>
+        <v>0.52460879229466095</v>
       </c>
       <c r="F7">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G7">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H7">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J7">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K7">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L7">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M7">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N7">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.2">
@@ -1249,40 +1243,40 @@
         <v>20</v>
       </c>
       <c r="B8">
-        <v>2.9013410386732699E-3</v>
+        <v>2.5624208731091099E-3</v>
       </c>
       <c r="C8">
-        <v>7.6338731447362302E-3</v>
+        <v>6.5201232498092601E-3</v>
       </c>
       <c r="D8">
-        <v>0.380061468623411</v>
+        <v>0.39300190731579698</v>
       </c>
       <c r="E8">
-        <v>0.70596180151452204</v>
+        <v>0.69645813340795504</v>
       </c>
       <c r="F8">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G8">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H8">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J8">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K8">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L8">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M8">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N8">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.2">
@@ -1290,40 +1284,40 @@
         <v>21</v>
       </c>
       <c r="B9">
-        <v>4.8024595884213796E-3</v>
+        <v>1.8201667593707299E-3</v>
       </c>
       <c r="C9">
-        <v>9.8401932003238293E-3</v>
+        <v>8.7665456662560405E-3</v>
       </c>
       <c r="D9">
-        <v>0.48804525385368802</v>
+        <v>0.20762645044750899</v>
       </c>
       <c r="E9">
-        <v>0.62825051566802403</v>
+        <v>0.83660105220569203</v>
       </c>
       <c r="F9">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G9">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H9">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J9">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K9">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L9">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M9">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N9">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -1331,40 +1325,40 @@
         <v>22</v>
       </c>
       <c r="B10">
-        <v>4.6465568325126097E-3</v>
+        <v>3.20221198246651E-3</v>
       </c>
       <c r="C10">
-        <v>7.3126759357452498E-3</v>
+        <v>6.5401001696195303E-3</v>
       </c>
       <c r="D10">
-        <v>0.63541128765185295</v>
+        <v>0.48962736034864102</v>
       </c>
       <c r="E10">
-        <v>0.52887112053382501</v>
+        <v>0.62714048679378498</v>
       </c>
       <c r="F10">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G10">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H10">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J10">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K10">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L10">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M10">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N10">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
@@ -1372,40 +1366,40 @@
         <v>23</v>
       </c>
       <c r="B11">
-        <v>-1.6368434036333E-3</v>
+        <v>-2.6801801033991702E-3</v>
       </c>
       <c r="C11">
-        <v>8.3770934983373405E-3</v>
+        <v>7.6517765454167299E-3</v>
       </c>
       <c r="D11">
-        <v>-0.19539514557861501</v>
+        <v>-0.35026899798904199</v>
       </c>
       <c r="E11">
-        <v>0.84609807688836203</v>
+        <v>0.72802159504011299</v>
       </c>
       <c r="F11">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G11">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H11">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J11">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K11">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L11">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M11">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N11">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -1413,40 +1407,40 @@
         <v>24</v>
       </c>
       <c r="B12">
-        <v>1.1475564748786001E-2</v>
+        <v>5.8898695409379002E-3</v>
       </c>
       <c r="C12">
-        <v>8.2544153210585697E-3</v>
+        <v>8.1677891538304691E-3</v>
       </c>
       <c r="D12">
-        <v>1.3902335056378401</v>
+        <v>0.72110940059902495</v>
       </c>
       <c r="E12">
-        <v>0.17234188333218101</v>
+        <v>0.475143044610635</v>
       </c>
       <c r="F12">
-        <v>0.17661697106037</v>
+        <v>0.176508258988853</v>
       </c>
       <c r="G12">
-        <v>9.2636152825865903E-2</v>
+        <v>0.10145940828606601</v>
       </c>
       <c r="H12">
-        <v>1.0669023858723701E-3</v>
+        <v>5.3808729647318899E-3</v>
       </c>
       <c r="J12">
-        <v>0.15947475542834</v>
+        <v>0.16026499101876299</v>
       </c>
       <c r="K12">
-        <v>171197</v>
+        <v>195468</v>
       </c>
       <c r="L12">
-        <v>-127690.70971955699</v>
+        <v>-145456.38124179401</v>
       </c>
       <c r="M12">
-        <v>31570.6259734388</v>
+        <v>20803.9408441575</v>
       </c>
       <c r="N12">
-        <v>79691.354859778396</v>
+        <v>89055.190620896901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>